<commit_message>
updated gui with CRUD
</commit_message>
<xml_diff>
--- a/record management project tracker.xlsx
+++ b/record management project tracker.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="200" documentId="8_{8B4BF8EB-79CE-4BEC-B0E9-733B2427CFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7B73464-A9C3-473F-AFEE-233EF55E11C0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="1785" windowWidth="14483" windowHeight="10388" xr2:uid="{51F1D3F4-E550-4DF2-AD77-01F7E648FC43}"/>
+    <workbookView xWindow="0" yWindow="1785" windowWidth="14483" windowHeight="10388" activeTab="1" xr2:uid="{51F1D3F4-E550-4DF2-AD77-01F7E648FC43}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -1288,11 +1288,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18DF439-6D05-4098-BFC2-8686C7AEBD88}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="56" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1606,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4DE54A-23BC-4E3B-9080-E3CAB6F72707}">
   <dimension ref="A2:A5"/>
   <sheetViews>
-    <sheetView zoomScale="56" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>